<commit_message>
further work on BDO and lipidcane biodiesel pretreatment
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_0.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_0.xlsx
@@ -52,7 +52,7 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Stream-lipidcane</t>
+    <t>Stream-sugarcane</t>
   </si>
   <si>
     <t>Stream-ethanol</t>
@@ -73,7 +73,7 @@
     <t>Lipid retention [%]</t>
   </si>
   <si>
-    <t>Additional lipid extraction efficiency [%]</t>
+    <t>Bagasse lipid extraction efficiency [%]</t>
   </si>
   <si>
     <t>Capacity [ton/hr]</t>
@@ -515,25 +515,22 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>0.469686006744027</v>
-      </c>
-      <c r="D4">
-        <v>0.9729738758955035</v>
+        <v>0.03827795694892373</v>
       </c>
       <c r="E4">
-        <v>-0.9701315925263702</v>
+        <v>-0.06061201530038251</v>
       </c>
       <c r="F4">
-        <v>0.8568704354817419</v>
+        <v>-0.06181354533863348</v>
       </c>
       <c r="H4">
-        <v>0.6314636458545834</v>
+        <v>-0.06061201530038251</v>
       </c>
       <c r="I4">
-        <v>0.6020103440413761</v>
+        <v>-0.08235205880147006</v>
       </c>
       <c r="J4">
-        <v>-0.948054951186682</v>
+        <v>-0.1558450909518538</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -542,25 +539,22 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>-0.06856645026580106</v>
-      </c>
-      <c r="D5">
-        <v>-0.06135134940539762</v>
+        <v>0.02411910297757444</v>
       </c>
       <c r="E5">
-        <v>0.04476104304417217</v>
+        <v>0.1472931823295582</v>
       </c>
       <c r="F5">
-        <v>-0.0645872343489374</v>
+        <v>0.1326213155328883</v>
       </c>
       <c r="H5">
-        <v>-0.05626409705638823</v>
+        <v>0.1412060301507538</v>
       </c>
       <c r="I5">
-        <v>-0.07523521294085177</v>
+        <v>0.08803720093002328</v>
       </c>
       <c r="J5">
-        <v>0.07836585971427537</v>
+        <v>0.01807414841114307</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -569,25 +563,22 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>-0.0457191268765075</v>
-      </c>
-      <c r="D6">
-        <v>-0.03995756783027132</v>
+        <v>-0.003130578264456612</v>
       </c>
       <c r="E6">
-        <v>0.05135809343237372</v>
+        <v>-0.05566489162229056</v>
       </c>
       <c r="F6">
-        <v>-0.02090427561710247</v>
+        <v>-0.06832970824270607</v>
       </c>
       <c r="H6">
-        <v>0.002044808179232717</v>
+        <v>-0.05884647116177905</v>
       </c>
       <c r="I6">
-        <v>0.01427976911907648</v>
+        <v>-0.06873471836795922</v>
       </c>
       <c r="J6">
-        <v>0.02807204408059924</v>
+        <v>-0.004111647505597405</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -596,25 +587,22 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>0.0738565514262057</v>
-      </c>
-      <c r="D7">
-        <v>0.2129084996339985</v>
+        <v>0.083625590639766</v>
       </c>
       <c r="E7">
-        <v>0.1343058812235249</v>
+        <v>0.7678016950423762</v>
       </c>
       <c r="F7">
-        <v>0.4336061824247297</v>
+        <v>0.7849681242031051</v>
       </c>
       <c r="H7">
-        <v>0.6220980403921615</v>
+        <v>0.7736998424960625</v>
       </c>
       <c r="I7">
-        <v>0.8119081756327026</v>
+        <v>0.9997449936248407</v>
       </c>
       <c r="J7">
-        <v>-0.07270629224707335</v>
+        <v>0.2469411090268892</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -625,25 +613,22 @@
         <v>21</v>
       </c>
       <c r="C8">
-        <v>0.4777799911199645</v>
-      </c>
-      <c r="D8">
-        <v>0.05745373381493526</v>
+        <v>0.9619410485262132</v>
       </c>
       <c r="E8">
-        <v>-0.05478703514814059</v>
+        <v>0.03280582014550364</v>
       </c>
       <c r="F8">
-        <v>0.05835306541226164</v>
+        <v>0.02794869871746794</v>
       </c>
       <c r="H8">
-        <v>0.04938307753231013</v>
+        <v>0.03044326108152704</v>
       </c>
       <c r="I8">
-        <v>0.01158167832671331</v>
+        <v>0.04204005100127504</v>
       </c>
       <c r="J8">
-        <v>-0.03891703237874738</v>
+        <v>0.02033172940199461</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -654,25 +639,22 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>0.6497782151128605</v>
-      </c>
-      <c r="D9">
-        <v>0.0387185868743475</v>
+        <v>-0.01385134628365709</v>
       </c>
       <c r="E9">
-        <v>-0.04711986847947391</v>
+        <v>-0.02015900397509938</v>
       </c>
       <c r="F9">
-        <v>0.02780353521414086</v>
+        <v>-0.02118802970074252</v>
       </c>
       <c r="H9">
-        <v>0.001790503162012648</v>
+        <v>-0.01914647866196655</v>
       </c>
       <c r="I9">
-        <v>0.03221062484249937</v>
+        <v>0.02138603465086627</v>
       </c>
       <c r="J9">
-        <v>-0.05941415434277044</v>
+        <v>-0.007806280050758446</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -683,25 +665,22 @@
         <v>22</v>
       </c>
       <c r="C10">
-        <v>-0.01469420277681111</v>
-      </c>
-      <c r="D10">
-        <v>-0.01833684134736539</v>
+        <v>0.113422335558389</v>
       </c>
       <c r="E10">
-        <v>0.05814013656054624</v>
+        <v>-0.002806570164254107</v>
       </c>
       <c r="F10">
-        <v>0.007844095376381505</v>
+        <v>-0.01432985824645617</v>
       </c>
       <c r="H10">
-        <v>0.0366690746762987</v>
+        <v>-0.00570014250356259</v>
       </c>
       <c r="I10">
-        <v>0.01283333133332533</v>
+        <v>-0.03298732468311708</v>
       </c>
       <c r="J10">
-        <v>0.02931429098749356</v>
+        <v>0.04264652994678374</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -712,25 +691,22 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>0.1588618194472778</v>
-      </c>
-      <c r="D11">
-        <v>0.01715978063912256</v>
+        <v>0.04565964149103728</v>
       </c>
       <c r="E11">
-        <v>-0.01255099420397681</v>
+        <v>0.1034230855771394</v>
       </c>
       <c r="F11">
-        <v>0.01800381601526406</v>
+        <v>0.09427285682142056</v>
       </c>
       <c r="H11">
-        <v>0.01403669614678459</v>
+        <v>0.102137553438836</v>
       </c>
       <c r="I11">
-        <v>0.01338379753519014</v>
+        <v>0.1267321683042076</v>
       </c>
       <c r="J11">
-        <v>-0.02329937754456749</v>
+        <v>0.04857549264867127</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -739,25 +715,22 @@
         <v>24</v>
       </c>
       <c r="C12">
-        <v>0.1802091368365473</v>
-      </c>
-      <c r="D12">
-        <v>0.2072832611330445</v>
+        <v>0.0834455861396535</v>
       </c>
       <c r="E12">
-        <v>0.06079483517934071</v>
+        <v>0.5355283882097053</v>
       </c>
       <c r="F12">
-        <v>0.3522097608390433</v>
+        <v>0.5153573839345984</v>
       </c>
       <c r="H12">
-        <v>0.4839817119268477</v>
+        <v>0.5315637890947275</v>
       </c>
       <c r="I12">
-        <v>0.01158916635666543</v>
+        <v>-0.09208580214505364</v>
       </c>
       <c r="J12">
-        <v>-0.04487338549607795</v>
+        <v>-0.1507861594623875</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -766,25 +739,22 @@
         <v>25</v>
       </c>
       <c r="C13">
-        <v>-0.280999555998224</v>
-      </c>
-      <c r="D13">
-        <v>0.01571075084300337</v>
+        <v>-0.2088097202430061</v>
       </c>
       <c r="E13">
-        <v>-0.04429995319981279</v>
+        <v>0.0003735093377334434</v>
       </c>
       <c r="F13">
-        <v>-0.003241356965427862</v>
+        <v>0.007227180679516989</v>
       </c>
       <c r="H13">
-        <v>-0.02851585806343225</v>
+        <v>0.001819545488637216</v>
       </c>
       <c r="I13">
-        <v>-0.04017625670502682</v>
+        <v>0.06154353858846472</v>
       </c>
       <c r="J13">
-        <v>-0.03090487583114723</v>
+        <v>-0.04711894039477304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>